<commit_message>
updated masses for 11 probes
</commit_message>
<xml_diff>
--- a/data/desgn_params.xlsx
+++ b/data/desgn_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="PRIMARY INPUTS" sheetId="6" r:id="rId1"/>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +560,7 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>2142</v>
+        <v>2252</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -843,7 +843,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B8">
         <f>'PRIMARY INPUTS'!B2</f>
-        <v>2142</v>
+        <v>2252</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Progress in final report
</commit_message>
<xml_diff>
--- a/data/desgn_params.xlsx
+++ b/data/desgn_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="PRIMARY INPUTS" sheetId="6" r:id="rId1"/>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +560,7 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>2252</v>
+        <v>2760</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
         <v>40</v>
       </c>
       <c r="B3">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -601,8 +601,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B8">
         <f>'PRIMARY INPUTS'!B2</f>
-        <v>2252</v>
+        <v>2760</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="B2">
         <f>'PRIMARY INPUTS'!B3</f>
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
desgn_params updated with report tables
</commit_message>
<xml_diff>
--- a/data/desgn_params.xlsx
+++ b/data/desgn_params.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexisPC\PycharmProjects\DSE-Mars-Reveal\project\subsystems_design\AOCS\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lmaio\Nextcloud\TU Delft\2019-2020\DSE-Mars-Reveal\project\subsystems_design\AOCS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772D630F-8DA0-423B-9844-231603290CA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="25560" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="25560" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="PRIMARY INPUTS" sheetId="6" r:id="rId1"/>
-    <sheet name="hardware" sheetId="3" r:id="rId2"/>
-    <sheet name="orb_mission" sheetId="1" r:id="rId3"/>
-    <sheet name="orb_props" sheetId="2" r:id="rId4"/>
-    <sheet name="probe_props" sheetId="4" r:id="rId5"/>
-    <sheet name="probe_mission" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId2"/>
+    <sheet name="hardware" sheetId="3" r:id="rId3"/>
+    <sheet name="orb_mission" sheetId="1" r:id="rId4"/>
+    <sheet name="orb_props" sheetId="2" r:id="rId5"/>
+    <sheet name="probe_props" sheetId="4" r:id="rId6"/>
+    <sheet name="probe_mission" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>value</t>
   </si>
@@ -212,12 +212,36 @@
   </si>
   <si>
     <t>kg/m3</t>
+  </si>
+  <si>
+    <t>A m^2</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>solar array area</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>TTC earth pt array moi</t>
+  </si>
+  <si>
+    <t>m^4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
@@ -558,16 +582,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,7 +608,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="6">
-        <v>3284.166976</v>
+        <v>5438.66</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -614,6 +639,7 @@
         <v>17</v>
       </c>
     </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -621,7 +647,210 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>3000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <f>'PRIMARY INPUTS'!B2</f>
+        <v>5438.66</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.05</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10">
+        <v>7.8826000000000001</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <v>102.87</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S8"/>
   <sheetViews>
@@ -896,13 +1125,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,13 +1275,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1354,7 @@
       </c>
       <c r="B8">
         <f>'PRIMARY INPUTS'!B2</f>
-        <v>3284.166976</v>
+        <v>5438.66</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -1139,8 +1368,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1196,8 +1425,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
added option to use aerobraking alt for torque calcualtions
</commit_message>
<xml_diff>
--- a/data/desgn_params.xlsx
+++ b/data/desgn_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="25560" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="25560" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PRIMARY INPUTS" sheetId="6" r:id="rId1"/>
@@ -21,24 +21,17 @@
     <sheet name="probe_mission" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>value</t>
   </si>
@@ -220,10 +213,16 @@
     <t>years</t>
   </si>
   <si>
-    <t>solar array area</t>
-  </si>
-  <si>
-    <t>m^2</t>
+    <t>solar array mass</t>
+  </si>
+  <si>
+    <t>solar array radius</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>solar array thickness</t>
   </si>
   <si>
     <t>Operations</t>
@@ -232,10 +231,13 @@
     <t>Parameters</t>
   </si>
   <si>
-    <t>TTC earth pt array moi</t>
-  </si>
-  <si>
-    <t>m^4</t>
+    <t>TTC earth array mass</t>
+  </si>
+  <si>
+    <t>TTC earth array radius</t>
+  </si>
+  <si>
+    <t>TTC earth array height</t>
   </si>
 </sst>
 </file>
@@ -585,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -648,20 +650,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -807,10 +812,10 @@
         <v>60</v>
       </c>
       <c r="F10">
-        <v>7.8826000000000001</v>
+        <v>12.5</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -824,13 +829,13 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11">
-        <v>102.87</v>
+        <v>0.05</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -842,6 +847,48 @@
       </c>
       <c r="C12" t="s">
         <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13">
+        <v>45.3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14">
+        <v>0.75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +1328,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
iteration 2 with fully loaded probes
</commit_message>
<xml_diff>
--- a/data/desgn_params.xlsx
+++ b/data/desgn_params.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="25560" windowHeight="13020" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="25560" windowHeight="13020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PRIMARY INPUTS" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
   <si>
     <t>value</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>TTC earth array height</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>http://www.msss.com/mars/global_surveyor/mgs_msn_plan/section5/section5.html</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +280,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -292,10 +306,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -304,8 +319,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1174,10 +1191,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1202,7 @@
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1193,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1204,7 +1221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1218,7 +1235,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1232,40 +1249,50 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>3000</v>
+        <v>1200</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>B7/60</f>
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1300,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1287,12 +1314,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B10">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1300,13 +1327,16 @@
       <c r="D10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H10" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B11">
-        <v>120</v>
+        <v>600</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1316,8 +1346,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1326,7 +1359,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>